<commit_message>
feat(report): generar XLSX desde plantilla, export endpoint /api/time/report.xlsx
</commit_message>
<xml_diff>
--- a/Reporte Plantilla.xlsx
+++ b/Reporte Plantilla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\Zonagamer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larry\Downloads\Carsplay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A73A68-A86B-4987-A71D-AC1297902C82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1DE52C-A9C1-4885-8401-17088D236568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11295" xr2:uid="{AA21D85A-83E0-456A-9149-1789D8CD4271}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AA21D85A-83E0-456A-9149-1789D8CD4271}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Reporte del día:</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Empleado</t>
   </si>
   <si>
-    <t>Consola</t>
-  </si>
-  <si>
     <t>Dinero generado</t>
   </si>
   <si>
@@ -61,13 +58,22 @@
   </si>
   <si>
     <t>Tiempo</t>
+  </si>
+  <si>
+    <t>CARSPLAY</t>
+  </si>
+  <si>
+    <t>Carrito</t>
+  </si>
+  <si>
+    <t>Fecha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +102,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -106,7 +134,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4D248E"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -138,17 +166,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -172,65 +212,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>927124</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5F79847-3563-4966-AB0E-DC9244B7941F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="66675" y="152400"/>
-          <a:ext cx="4537099" cy="1485900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -268,7 +253,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -374,7 +359,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -516,7 +501,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -526,202 +511,210 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966D3468-F579-451C-B4F6-49978F6B38FE}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="84" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="5" width="24.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="4" max="5" width="24.5546875" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.109375" customWidth="1"/>
+    <col min="8" max="8" width="24.5546875" customWidth="1"/>
+    <col min="9" max="9" width="46.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-    </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="4" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="1:17" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="3" t="s">
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="12" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-    </row>
-    <row r="12" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="2" t="s">
+      <c r="H12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="I12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:D3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>